<commit_message>
update import price list
</commit_message>
<xml_diff>
--- a/public/downloads/sample_excels/price_lists_import_sample.xlsx
+++ b/public/downloads/sample_excels/price_lists_import_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\HSBR OneDrive\HSBR Apps\Projects\HSBR-APP\hsbr-apps-adminLTE\public\downloads\sample_excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3014018-ADD8-4C17-84D2-D529503704FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7018A6D-CEBB-4146-8E99-E99F3AF93B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{BEBF86B8-2F91-4EC2-8B46-CAF70645DC37}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>status</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>code</t>
-  </si>
-  <si>
-    <t>local_name</t>
   </si>
   <si>
     <t>group</t>
@@ -426,30 +423,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1589E59C-D970-41BA-BC8E-1FE887340269}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="13" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -466,13 +462,13 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
         <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -484,9 +480,6 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>